<commit_message>
Mejora de hipotesis nula
</commit_message>
<xml_diff>
--- a/AnovaExperimentacion.xlsx
+++ b/AnovaExperimentacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Esteban Gallo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Esteban Gallo\source\repos\Taller-Dise-o-Experimentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{34EE7273-5464-42A9-8567-61648E36FB24}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ABDC5093-E5B3-49FE-9A83-501FC660B123}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="1" xr2:uid="{5B3DDE98-DCD0-4CC9-A8FA-01F729F02502}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8811" activeTab="1" xr2:uid="{5B3DDE98-DCD0-4CC9-A8FA-01F729F02502}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="38">
   <si>
     <t/>
   </si>
@@ -91,18 +91,12 @@
     <t>Dentro de grupos</t>
   </si>
   <si>
-    <t>Alguno de los grupos comparados son distintos</t>
-  </si>
-  <si>
     <t>HI</t>
   </si>
   <si>
     <t>HO</t>
   </si>
   <si>
-    <t>Alguno de los grupos comparados son iguales</t>
-  </si>
-  <si>
     <t>&lt;0,05</t>
   </si>
   <si>
@@ -143,6 +137,9 @@
   </si>
   <si>
     <t>Conclusion: por analisis de medias y probando con una prueba anova, los factores comparados en un arreglo de 10^4 de forma ascendente, no se ve diferencia entre si,por lo cual no podemos decir en este caso que un RandomQuickSort es mejor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El promedio entre medias de ambos tratamientos son diferentes </t>
   </si>
 </sst>
 </file>
@@ -734,7 +731,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -774,17 +771,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -826,15 +812,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="36" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -849,18 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -899,42 +864,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="36" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -946,18 +875,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -996,39 +913,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1046,18 +930,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1112,24 +984,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1187,9 +1041,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1199,24 +1050,23 @@
     <xf numFmtId="166" fontId="6" fillId="4" borderId="39" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1226,9 +1076,172 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="36" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="36" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
@@ -1553,34 +1566,34 @@
       <selection activeCell="C47" sqref="C47:G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.05078125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.61328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="23.7">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:12" ht="24">
+      <c r="A3" s="125" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1603,7 +1616,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="22.8">
+    <row r="5" spans="1:12" ht="23.15">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -1627,11 +1640,11 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="22.8">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:12" ht="23.15">
+      <c r="A8" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="126" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1648,8 +1661,8 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="15"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="122"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1663,9 +1676,9 @@
         <v>1.728190000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="23.7">
-      <c r="A10" s="15"/>
-      <c r="B10" s="19"/>
+    <row r="10" spans="1:12" ht="24">
+      <c r="A10" s="122"/>
+      <c r="B10" s="126"/>
       <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
@@ -1705,17 +1718,17 @@
         <v>3.1268910740952068E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="23.7">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:12" ht="23.15">
+      <c r="A16" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="122"/>
       <c r="D16" s="2"/>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="123" t="s">
         <v>2</v>
       </c>
       <c r="I16" s="14" t="s">
@@ -1732,14 +1745,14 @@
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
       <c r="D17" s="2"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="122"/>
+      <c r="H17" s="124"/>
       <c r="I17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1753,8 +1766,8 @@
         <v>0.23828294999999983</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="35.1">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:18" ht="35.6">
+      <c r="A18" s="125" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1764,8 +1777,8 @@
         <v>5</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="17"/>
+      <c r="G18" s="122"/>
+      <c r="H18" s="124"/>
       <c r="I18" s="4" t="s">
         <v>5</v>
       </c>
@@ -1797,7 +1810,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:18" ht="22.8">
+    <row r="20" spans="1:18" ht="23.15">
       <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
@@ -1821,26 +1834,26 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="25" spans="1:18" ht="23.7">
-      <c r="A25" s="15" t="s">
+    <row r="25" spans="1:18" ht="24">
+      <c r="A25" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="122"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
+      <c r="I25" s="122"/>
+      <c r="J25" s="122"/>
       <c r="K25" s="2"/>
-      <c r="M25" s="15" t="s">
+      <c r="M25" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="N25" s="16" t="s">
+      <c r="N25" s="123" t="s">
         <v>2</v>
       </c>
       <c r="O25" s="14" t="s">
@@ -1857,23 +1870,23 @@
       </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="124"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="124"/>
       <c r="K26" s="2"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="17"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="124"/>
       <c r="O26" s="3" t="s">
         <v>4</v>
       </c>
@@ -1887,27 +1900,27 @@
         <v>7.4014221999999918</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="35.1">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:18" ht="35.6">
+      <c r="A27" s="125" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G27" s="2"/>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="125" t="s">
         <v>3</v>
       </c>
       <c r="I27" s="3" t="s">
@@ -1917,8 +1930,8 @@
         <v>5</v>
       </c>
       <c r="K27" s="2"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="17"/>
+      <c r="M27" s="122"/>
+      <c r="N27" s="124"/>
       <c r="O27" s="4" t="s">
         <v>5</v>
       </c>
@@ -1932,23 +1945,23 @@
         <v>8.0857375131463127E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="22.8">
+    <row r="28" spans="1:18" ht="23.15">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="16">
         <v>15.795131716125024</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="17">
         <v>1</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="18">
         <v>15.795131716125024</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="18">
         <v>2751.3190596526474</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="19">
         <v>0</v>
       </c>
       <c r="G28" s="2"/>
@@ -1969,21 +1982,21 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="1:18" ht="22.8">
+    <row r="29" spans="1:18" ht="23.15">
       <c r="A29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="20">
         <v>11.470379292470014</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="21">
         <v>1998</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="22">
         <v>5.7409305768118188E-3</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="2"/>
       <c r="H29" s="8" t="s">
         <v>7</v>
@@ -2000,15 +2013,15 @@
       <c r="A30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="25">
         <v>27.265511008595038</v>
       </c>
-      <c r="C30" s="31">
+      <c r="C30" s="26">
         <v>1999</v>
       </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="2"/>
       <c r="H30" s="11" t="s">
         <v>8</v>
@@ -2022,27 +2035,27 @@
       <c r="K30" s="2"/>
     </row>
     <row r="34" spans="1:19">
-      <c r="M34" s="15" t="s">
+      <c r="M34" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
+      <c r="N34" s="122"/>
+      <c r="O34" s="122"/>
+      <c r="P34" s="122"/>
+      <c r="Q34" s="122"/>
+      <c r="R34" s="122"/>
       <c r="S34" s="2"/>
     </row>
-    <row r="35" spans="1:19" ht="23.7">
-      <c r="A35" s="15" t="s">
+    <row r="35" spans="1:19" ht="24">
+      <c r="A35" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="122"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="123" t="s">
         <v>2</v>
       </c>
       <c r="G35" s="14" t="s">
@@ -2057,25 +2070,25 @@
       <c r="J35" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M35" s="16" t="s">
+      <c r="M35" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
+      <c r="N35" s="124"/>
+      <c r="O35" s="124"/>
+      <c r="P35" s="124"/>
+      <c r="Q35" s="124"/>
+      <c r="R35" s="124"/>
       <c r="S35" s="2"/>
     </row>
-    <row r="36" spans="1:19" ht="23.7">
-      <c r="A36" s="16" t="s">
+    <row r="36" spans="1:19" ht="24">
+      <c r="A36" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
+      <c r="B36" s="124"/>
+      <c r="C36" s="124"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="17"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="124"/>
       <c r="G36" s="3" t="s">
         <v>4</v>
       </c>
@@ -2088,19 +2101,19 @@
       <c r="J36" s="12">
         <v>962.03895065000086</v>
       </c>
-      <c r="M36" s="18" t="s">
+      <c r="M36" s="125" t="s">
         <v>0</v>
       </c>
       <c r="N36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O36" s="20" t="s">
+      <c r="O36" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="P36" s="20" t="s">
+      <c r="P36" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Q36" s="20" t="s">
+      <c r="Q36" s="15" t="s">
         <v>17</v>
       </c>
       <c r="R36" s="4" t="s">
@@ -2108,8 +2121,8 @@
       </c>
       <c r="S36" s="2"/>
     </row>
-    <row r="37" spans="1:19" ht="35.1">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:19" ht="35.6">
+      <c r="A37" s="125" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2119,8 +2132,8 @@
         <v>5</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="17"/>
+      <c r="E37" s="122"/>
+      <c r="F37" s="124"/>
       <c r="G37" s="4" t="s">
         <v>5</v>
       </c>
@@ -2136,24 +2149,24 @@
       <c r="M37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N37" s="21">
+      <c r="N37" s="16">
         <v>22344.329056898772</v>
       </c>
-      <c r="O37" s="22">
+      <c r="O37" s="17">
         <v>1</v>
       </c>
-      <c r="P37" s="23">
+      <c r="P37" s="18">
         <v>22344.329056898772</v>
       </c>
-      <c r="Q37" s="23">
+      <c r="Q37" s="18">
         <v>11766.199900161366</v>
       </c>
-      <c r="R37" s="24">
+      <c r="R37" s="19">
         <v>0</v>
       </c>
       <c r="S37" s="2"/>
     </row>
-    <row r="38" spans="1:19" ht="22.8">
+    <row r="38" spans="1:19" ht="23.15">
       <c r="A38" s="5" t="s">
         <v>6</v>
       </c>
@@ -2167,20 +2180,20 @@
       <c r="M38" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N38" s="25">
+      <c r="N38" s="20">
         <v>3794.2555654754333</v>
       </c>
-      <c r="O38" s="26">
+      <c r="O38" s="21">
         <v>1998</v>
       </c>
-      <c r="P38" s="27">
+      <c r="P38" s="22">
         <v>1.899026809547264</v>
       </c>
-      <c r="Q38" s="28"/>
-      <c r="R38" s="29"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="24"/>
       <c r="S38" s="2"/>
     </row>
-    <row r="39" spans="1:19" ht="22.8">
+    <row r="39" spans="1:19" ht="23.15">
       <c r="A39" s="8" t="s">
         <v>7</v>
       </c>
@@ -2194,15 +2207,15 @@
       <c r="M39" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N39" s="30">
+      <c r="N39" s="25">
         <v>26138.584622374205</v>
       </c>
-      <c r="O39" s="31">
+      <c r="O39" s="26">
         <v>1999</v>
       </c>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="32"/>
-      <c r="R39" s="33"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="28"/>
       <c r="S39" s="2"/>
     </row>
     <row r="40" spans="1:19">
@@ -2218,41 +2231,41 @@
       <c r="D40" s="2"/>
     </row>
     <row r="44" spans="1:19">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
+      <c r="C44" s="122"/>
+      <c r="D44" s="122"/>
+      <c r="E44" s="122"/>
+      <c r="F44" s="122"/>
+      <c r="G44" s="122"/>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:19">
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
+      <c r="C45" s="124"/>
+      <c r="D45" s="124"/>
+      <c r="E45" s="124"/>
+      <c r="F45" s="124"/>
+      <c r="G45" s="124"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:19" ht="23.7">
-      <c r="B46" s="18" t="s">
+    <row r="46" spans="1:19" ht="24">
+      <c r="B46" s="125" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="E46" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="15" t="s">
         <v>17</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -2264,57 +2277,78 @@
       <c r="B47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="21">
+      <c r="C47" s="16">
         <v>7516273.5230968921</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="17">
         <v>1</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E47" s="18">
         <v>7516273.5230968921</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="18">
         <v>0.68088794639577577</v>
       </c>
-      <c r="G47" s="24">
+      <c r="G47" s="19">
         <v>0.4093796362981551</v>
       </c>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:19" ht="22.8">
+    <row r="48" spans="1:19" ht="23.15">
       <c r="B48" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="25">
+      <c r="C48" s="20">
         <v>22055779631.056133</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D48" s="21">
         <v>1998</v>
       </c>
-      <c r="E48" s="27">
+      <c r="E48" s="22">
         <v>11038928.744272338</v>
       </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="29"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="24"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="30">
+      <c r="C49" s="25">
         <v>22063295904.579231</v>
       </c>
-      <c r="D49" s="31">
+      <c r="D49" s="26">
         <v>1999</v>
       </c>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="33"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="28"/>
       <c r="H49" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27"/>
+    <mergeCell ref="M25:M27"/>
+    <mergeCell ref="N25:N27"/>
+    <mergeCell ref="M34:R34"/>
+    <mergeCell ref="M35:R35"/>
+    <mergeCell ref="M36"/>
     <mergeCell ref="B44:G44"/>
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="B46"/>
@@ -2323,27 +2357,6 @@
     <mergeCell ref="A37"/>
     <mergeCell ref="E35:E37"/>
     <mergeCell ref="F35:F37"/>
-    <mergeCell ref="M25:M27"/>
-    <mergeCell ref="N25:N27"/>
-    <mergeCell ref="M34:R34"/>
-    <mergeCell ref="M35:R35"/>
-    <mergeCell ref="M36"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2353,1033 +2366,1033 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA92E38-629E-4F49-A95A-220CE5369EDD}">
   <dimension ref="A4:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="19.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.3125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1015625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7890625" customWidth="1"/>
+    <col min="1" max="1" width="19.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.3046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15" ht="14.7" thickBot="1"/>
+    <row r="4" spans="1:15" ht="15" thickBot="1"/>
     <row r="5" spans="1:15" ht="34.200000000000003" customHeight="1">
-      <c r="A5" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36"/>
-      <c r="I5" s="72" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="74"/>
+      <c r="A5" s="175" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="176"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="177"/>
+      <c r="I5" s="151" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="152"/>
+      <c r="K5" s="152"/>
+      <c r="L5" s="152"/>
+      <c r="M5" s="152"/>
+      <c r="N5" s="152"/>
+      <c r="O5" s="153"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="40"/>
-      <c r="I6" s="75" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="I6" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="76" t="s">
+      <c r="K6" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="78"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="149">
+      <c r="B7" s="94">
         <v>4.2996999999999966E-3</v>
       </c>
-      <c r="C7" s="149">
+      <c r="C7" s="94">
         <v>3.0264100000000002E-2</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="40"/>
-      <c r="I7" s="156" t="s">
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="I7" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="157">
+      <c r="J7" s="102">
         <v>0.1494146999999999</v>
       </c>
-      <c r="K7" s="157">
+      <c r="K7" s="102">
         <v>0.32715120000000059</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="78"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="52"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="150">
+      <c r="B8" s="95">
         <v>4.2228108211511491E-5</v>
       </c>
-      <c r="C8" s="150">
+      <c r="C8" s="95">
         <v>5.1265854130207373E-4</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="40"/>
-      <c r="I8" s="156" t="s">
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="32"/>
+      <c r="I8" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="158">
+      <c r="J8" s="103">
         <v>1.5218008778489455E-3</v>
       </c>
-      <c r="K8" s="158">
+      <c r="K8" s="103">
         <v>3.0275374880918996E-3</v>
       </c>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="78"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="52"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9" s="34">
         <f>B7-1.96*B8</f>
         <v>4.2169329079054345E-3</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="34">
         <f>C7-1.96*C8</f>
         <v>2.9259289259047937E-2</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="I9" s="156" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32"/>
+      <c r="I9" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="79">
+      <c r="J9" s="53">
         <f>J7-1.96*J8</f>
         <v>0.14643197027941596</v>
       </c>
-      <c r="K9" s="79">
+      <c r="K9" s="53">
         <f>K7-1.96*K8</f>
         <v>0.32121722652334045</v>
       </c>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
-      <c r="N9" s="77"/>
-      <c r="O9" s="78"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="52"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10" s="34">
         <f>B7+1.96*B8</f>
         <v>4.3824670920945587E-3</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="34">
         <f>C7+1.96*C8</f>
         <v>3.1268910740952068E-2</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="I10" s="156" t="s">
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32"/>
+      <c r="I10" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="79">
+      <c r="J10" s="53">
         <f>J7+1.96*J8</f>
         <v>0.15239742972058384</v>
       </c>
-      <c r="K10" s="79">
+      <c r="K10" s="53">
         <f>K7+1.96*K8</f>
         <v>0.33308517347666072</v>
       </c>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="78"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="52"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="43"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="77"/>
-      <c r="N11" s="77"/>
-      <c r="O11" s="78"/>
-    </row>
-    <row r="12" spans="1:15" ht="14.7" thickBot="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
-      <c r="N12" s="77"/>
-      <c r="O12" s="78"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="32"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="52"/>
+    </row>
+    <row r="12" spans="1:15" ht="15" thickBot="1">
+      <c r="A12" s="35"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="52"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="169" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="40"/>
-      <c r="I13" s="81" t="s">
+      <c r="B13" s="170"/>
+      <c r="C13" s="170"/>
+      <c r="D13" s="170"/>
+      <c r="E13" s="170"/>
+      <c r="F13" s="171"/>
+      <c r="G13" s="32"/>
+      <c r="I13" s="154" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="78"/>
+      <c r="J13" s="155"/>
+      <c r="K13" s="155"/>
+      <c r="L13" s="155"/>
+      <c r="M13" s="155"/>
+      <c r="N13" s="156"/>
+      <c r="O13" s="52"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="172" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="40"/>
-      <c r="I14" s="84" t="s">
+      <c r="B14" s="173"/>
+      <c r="C14" s="173"/>
+      <c r="D14" s="173"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="174"/>
+      <c r="G14" s="32"/>
+      <c r="I14" s="157" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="L14" s="85"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="78"/>
-    </row>
-    <row r="15" spans="1:15" ht="43.2">
-      <c r="A15" s="50" t="s">
+      <c r="J14" s="158"/>
+      <c r="K14" s="158"/>
+      <c r="L14" s="158"/>
+      <c r="M14" s="158"/>
+      <c r="N14" s="159"/>
+      <c r="O14" s="52"/>
+    </row>
+    <row r="15" spans="1:15" ht="43.75">
+      <c r="A15" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="53" t="s">
+      <c r="F15" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="87" t="s">
+      <c r="G15" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="88" t="s">
+      <c r="J15" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="89" t="s">
+      <c r="K15" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="89" t="s">
+      <c r="L15" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="M15" s="89" t="s">
+      <c r="M15" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="90" t="s">
+      <c r="N15" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="O15" s="78" t="s">
-        <v>28</v>
+      <c r="O15" s="52" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="55">
+      <c r="B16" s="41">
         <v>0.33707503367999819</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="42">
         <v>1</v>
       </c>
-      <c r="D16" s="57">
+      <c r="D16" s="43">
         <v>0.33707503367999819</v>
       </c>
-      <c r="E16" s="57">
+      <c r="E16" s="43">
         <v>2547.7890755071285</v>
       </c>
-      <c r="F16" s="151">
+      <c r="F16" s="96">
         <v>0</v>
       </c>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="60">
+        <v>15.795131716125024</v>
+      </c>
+      <c r="K16" s="61">
+        <v>1</v>
+      </c>
+      <c r="L16" s="62">
+        <v>15.795131716125024</v>
+      </c>
+      <c r="M16" s="62">
+        <v>2751.3190596526474</v>
+      </c>
+      <c r="N16" s="107">
+        <v>0</v>
+      </c>
+      <c r="O16" s="52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="29.15">
+      <c r="A17" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="45">
+        <v>0.26433739110000043</v>
+      </c>
+      <c r="C17" s="46">
+        <v>1998</v>
+      </c>
+      <c r="D17" s="47">
+        <v>1.3230099654654677E-4</v>
+      </c>
+      <c r="E17" s="48"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="32"/>
+      <c r="I17" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="64">
+        <v>11.470379292470014</v>
+      </c>
+      <c r="K17" s="65">
+        <v>1998</v>
+      </c>
+      <c r="L17" s="66">
+        <v>5.7409305768118188E-3</v>
+      </c>
+      <c r="M17" s="67"/>
+      <c r="N17" s="108"/>
+      <c r="O17" s="52"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" thickBot="1">
+      <c r="A18" s="104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="105">
+        <v>0.60141242477999857</v>
+      </c>
+      <c r="C18" s="98">
+        <v>1999</v>
+      </c>
+      <c r="D18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="32"/>
+      <c r="I18" s="106" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="109">
+        <v>27.265511008595038</v>
+      </c>
+      <c r="K18" s="110">
+        <v>1999</v>
+      </c>
+      <c r="L18" s="111"/>
+      <c r="M18" s="111"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="52"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="187" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="32"/>
+      <c r="I19" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="52"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="187" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+      <c r="I20" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="52"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="184" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="185"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="185"/>
+      <c r="E21" s="185"/>
+      <c r="F21" s="185"/>
+      <c r="G21" s="186"/>
+      <c r="I21" s="160" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="161"/>
+      <c r="K21" s="161"/>
+      <c r="L21" s="161"/>
+      <c r="M21" s="161"/>
+      <c r="N21" s="161"/>
+      <c r="O21" s="162"/>
+    </row>
+    <row r="22" spans="1:15" ht="14.4" customHeight="1">
+      <c r="A22" s="178" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="91" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="92">
-        <v>15.795131716125024</v>
-      </c>
-      <c r="K16" s="93">
-        <v>1</v>
-      </c>
-      <c r="L16" s="94">
-        <v>15.795131716125024</v>
-      </c>
-      <c r="M16" s="94">
-        <v>2751.3190596526474</v>
-      </c>
-      <c r="N16" s="162">
-        <v>0</v>
-      </c>
-      <c r="O16" s="78" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="59">
-        <v>0.26433739110000043</v>
-      </c>
-      <c r="C17" s="60">
-        <v>1998</v>
-      </c>
-      <c r="D17" s="61">
-        <v>1.3230099654654677E-4</v>
-      </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="152"/>
-      <c r="G17" s="40"/>
-      <c r="I17" s="95" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="96">
-        <v>11.470379292470014</v>
-      </c>
-      <c r="K17" s="97">
-        <v>1998</v>
-      </c>
-      <c r="L17" s="98">
-        <v>5.7409305768118188E-3</v>
-      </c>
-      <c r="M17" s="99"/>
-      <c r="N17" s="163"/>
-      <c r="O17" s="78"/>
-    </row>
-    <row r="18" spans="1:15" ht="14.7" thickBot="1">
-      <c r="A18" s="159" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="160">
-        <v>0.60141242477999857</v>
-      </c>
-      <c r="C18" s="153">
-        <v>1999</v>
-      </c>
-      <c r="D18" s="154"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="155"/>
-      <c r="G18" s="40"/>
-      <c r="I18" s="161" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="164">
-        <v>27.265511008595038</v>
-      </c>
-      <c r="K18" s="165">
-        <v>1999</v>
-      </c>
-      <c r="L18" s="166"/>
-      <c r="M18" s="166"/>
-      <c r="N18" s="167"/>
-      <c r="O18" s="78"/>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
-      <c r="I19" s="80" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="77" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="77"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="78"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="I20" s="80" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" s="77"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="77"/>
-      <c r="N20" s="77"/>
-      <c r="O20" s="78"/>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="63" t="s">
+      <c r="B22" s="179"/>
+      <c r="C22" s="179"/>
+      <c r="D22" s="179"/>
+      <c r="E22" s="179"/>
+      <c r="F22" s="179"/>
+      <c r="G22" s="180"/>
+      <c r="I22" s="163" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="164"/>
+      <c r="K22" s="164"/>
+      <c r="L22" s="164"/>
+      <c r="M22" s="164"/>
+      <c r="N22" s="164"/>
+      <c r="O22" s="165"/>
+    </row>
+    <row r="23" spans="1:15" ht="31.3" customHeight="1" thickBot="1">
+      <c r="A23" s="181"/>
+      <c r="B23" s="182"/>
+      <c r="C23" s="182"/>
+      <c r="D23" s="182"/>
+      <c r="E23" s="182"/>
+      <c r="F23" s="182"/>
+      <c r="G23" s="183"/>
+      <c r="I23" s="166"/>
+      <c r="J23" s="167"/>
+      <c r="K23" s="167"/>
+      <c r="L23" s="167"/>
+      <c r="M23" s="167"/>
+      <c r="N23" s="167"/>
+      <c r="O23" s="168"/>
+    </row>
+    <row r="25" spans="1:15" ht="15" thickBot="1"/>
+    <row r="26" spans="1:15">
+      <c r="A26" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="65"/>
-      <c r="I21" s="100" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="101"/>
-      <c r="K21" s="101"/>
-      <c r="L21" s="101"/>
-      <c r="M21" s="101"/>
-      <c r="N21" s="101"/>
-      <c r="O21" s="102"/>
-    </row>
-    <row r="22" spans="1:15" ht="14.4" customHeight="1">
-      <c r="A22" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="68"/>
-      <c r="I22" s="168" t="s">
-        <v>33</v>
-      </c>
-      <c r="J22" s="103"/>
-      <c r="K22" s="103"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
-      <c r="N22" s="103"/>
-      <c r="O22" s="104"/>
-    </row>
-    <row r="23" spans="1:15" ht="14.7" thickBot="1">
-      <c r="A23" s="69"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="71"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="106"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="106"/>
-      <c r="N23" s="106"/>
-      <c r="O23" s="107"/>
-    </row>
-    <row r="25" spans="1:15" ht="14.7" thickBot="1"/>
-    <row r="26" spans="1:15">
-      <c r="A26" s="108" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="109"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="109"/>
-      <c r="G26" s="110"/>
-      <c r="I26" s="184" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="185"/>
-      <c r="K26" s="185"/>
-      <c r="L26" s="185"/>
-      <c r="M26" s="185"/>
-      <c r="N26" s="185"/>
-      <c r="O26" s="186"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="135"/>
+      <c r="I26" s="127" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="128"/>
+      <c r="K26" s="128"/>
+      <c r="L26" s="128"/>
+      <c r="M26" s="128"/>
+      <c r="N26" s="128"/>
+      <c r="O26" s="129"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="111" t="s">
+      <c r="A27" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="111" t="s">
+      <c r="B27" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="112" t="s">
+      <c r="C27" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="113"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="113"/>
-      <c r="G27" s="114"/>
-      <c r="I27" s="175" t="s">
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="71"/>
+      <c r="I27" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="176" t="s">
+      <c r="J27" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="K27" s="176" t="s">
+      <c r="K27" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="L27" s="176"/>
-      <c r="M27" s="176"/>
-      <c r="N27" s="176"/>
-      <c r="O27" s="177"/>
+      <c r="L27" s="117"/>
+      <c r="M27" s="117"/>
+      <c r="N27" s="117"/>
+      <c r="O27" s="118"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="169" t="s">
+      <c r="A28" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="115">
+      <c r="B28" s="72">
         <v>10.74390100000001</v>
       </c>
-      <c r="C28" s="115">
+      <c r="C28" s="72">
         <v>4.0589434000000049</v>
       </c>
-      <c r="D28" s="113"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="113"/>
-      <c r="G28" s="114"/>
-      <c r="I28" s="175" t="s">
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="71"/>
+      <c r="I28" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="J28" s="176">
+      <c r="J28" s="117">
         <v>900.7353066999998</v>
       </c>
-      <c r="K28" s="176">
+      <c r="K28" s="117">
         <v>1023.3425946000018</v>
       </c>
-      <c r="L28" s="176"/>
-      <c r="M28" s="176"/>
-      <c r="N28" s="176"/>
-      <c r="O28" s="177"/>
+      <c r="L28" s="117"/>
+      <c r="M28" s="117"/>
+      <c r="N28" s="117"/>
+      <c r="O28" s="118"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="169" t="s">
+      <c r="A29" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="116">
+      <c r="B29" s="73">
         <v>5.7457501750305784E-2</v>
       </c>
-      <c r="C29" s="116">
+      <c r="C29" s="73">
         <v>2.2286523095991169E-2</v>
       </c>
-      <c r="D29" s="113"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="113"/>
-      <c r="G29" s="114"/>
-      <c r="I29" s="175" t="s">
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="I29" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="J29" s="176">
+      <c r="J29" s="117">
         <v>148.54816930833306</v>
       </c>
-      <c r="K29" s="176">
+      <c r="K29" s="117">
         <v>3.3613812172229496</v>
       </c>
-      <c r="L29" s="176"/>
-      <c r="M29" s="176"/>
-      <c r="N29" s="176"/>
-      <c r="O29" s="177"/>
+      <c r="L29" s="117"/>
+      <c r="M29" s="117"/>
+      <c r="N29" s="117"/>
+      <c r="O29" s="118"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="169" t="s">
+      <c r="A30" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="117">
+      <c r="B30" s="74">
         <f>B28-1.96*B29</f>
         <v>10.63128429656941</v>
       </c>
-      <c r="C30" s="117">
+      <c r="C30" s="74">
         <f>C28-1.96*C29</f>
         <v>4.0152618147318622</v>
       </c>
-      <c r="D30" s="113"/>
-      <c r="E30" s="113"/>
-      <c r="F30" s="113"/>
-      <c r="G30" s="114"/>
-      <c r="I30" s="175" t="s">
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="71"/>
+      <c r="I30" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="J30" s="176">
+      <c r="J30" s="117">
         <f>J28-1.96*J29</f>
         <v>609.580894855667</v>
       </c>
-      <c r="K30" s="176">
+      <c r="K30" s="117">
         <f>K28-1.96*K29</f>
         <v>1016.7542874142448</v>
       </c>
-      <c r="L30" s="176"/>
-      <c r="M30" s="176"/>
-      <c r="N30" s="176"/>
-      <c r="O30" s="177"/>
+      <c r="L30" s="117"/>
+      <c r="M30" s="117"/>
+      <c r="N30" s="117"/>
+      <c r="O30" s="118"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="169" t="s">
+      <c r="A31" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="117">
+      <c r="B31" s="74">
         <f>B28+1.96*B29</f>
         <v>10.85651770343061</v>
       </c>
-      <c r="C31" s="117">
+      <c r="C31" s="74">
         <f>C28+1.96*C29</f>
         <v>4.1026249852681476</v>
       </c>
-      <c r="D31" s="113"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="113"/>
-      <c r="G31" s="114"/>
-      <c r="I31" s="175" t="s">
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
+      <c r="I31" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="J31" s="176">
+      <c r="J31" s="117">
         <f>J28+1.96*J29</f>
         <v>1191.8897185443325</v>
       </c>
-      <c r="K31" s="176">
+      <c r="K31" s="117">
         <f>K28+1.96*K29</f>
         <v>1029.9309017857588</v>
       </c>
-      <c r="L31" s="176"/>
-      <c r="M31" s="176"/>
-      <c r="N31" s="176"/>
-      <c r="O31" s="177"/>
+      <c r="L31" s="117"/>
+      <c r="M31" s="117"/>
+      <c r="N31" s="117"/>
+      <c r="O31" s="118"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="118"/>
-      <c r="B32" s="113"/>
-      <c r="C32" s="113"/>
-      <c r="D32" s="113"/>
-      <c r="E32" s="113"/>
-      <c r="F32" s="113"/>
-      <c r="G32" s="114"/>
-      <c r="I32" s="175"/>
-      <c r="J32" s="176"/>
-      <c r="K32" s="176"/>
-      <c r="L32" s="176"/>
-      <c r="M32" s="176"/>
-      <c r="N32" s="176"/>
-      <c r="O32" s="177"/>
-    </row>
-    <row r="33" spans="1:15" ht="14.7" thickBot="1">
-      <c r="A33" s="118"/>
-      <c r="B33" s="113"/>
-      <c r="C33" s="113"/>
-      <c r="D33" s="113"/>
-      <c r="E33" s="113"/>
-      <c r="F33" s="113"/>
-      <c r="G33" s="114"/>
-      <c r="I33" s="175"/>
-      <c r="J33" s="176"/>
-      <c r="K33" s="176"/>
-      <c r="L33" s="176"/>
-      <c r="M33" s="176"/>
-      <c r="N33" s="176"/>
-      <c r="O33" s="177"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="71"/>
+      <c r="I32" s="116"/>
+      <c r="J32" s="117"/>
+      <c r="K32" s="117"/>
+      <c r="L32" s="117"/>
+      <c r="M32" s="117"/>
+      <c r="N32" s="117"/>
+      <c r="O32" s="118"/>
+    </row>
+    <row r="33" spans="1:15" ht="15" thickBot="1">
+      <c r="A33" s="75"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
+      <c r="I33" s="116"/>
+      <c r="J33" s="117"/>
+      <c r="K33" s="117"/>
+      <c r="L33" s="117"/>
+      <c r="M33" s="117"/>
+      <c r="N33" s="117"/>
+      <c r="O33" s="118"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="136" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="120"/>
-      <c r="C34" s="120"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="114"/>
-      <c r="I34" s="184" t="s">
+      <c r="B34" s="137"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="137"/>
+      <c r="E34" s="137"/>
+      <c r="F34" s="138"/>
+      <c r="G34" s="71"/>
+      <c r="I34" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="J34" s="185"/>
-      <c r="K34" s="185"/>
-      <c r="L34" s="185"/>
-      <c r="M34" s="185"/>
-      <c r="N34" s="186"/>
-      <c r="O34" s="177"/>
+      <c r="J34" s="128"/>
+      <c r="K34" s="128"/>
+      <c r="L34" s="128"/>
+      <c r="M34" s="128"/>
+      <c r="N34" s="129"/>
+      <c r="O34" s="118"/>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" s="122" t="s">
+      <c r="A35" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="123"/>
-      <c r="C35" s="123"/>
-      <c r="D35" s="123"/>
-      <c r="E35" s="123"/>
-      <c r="F35" s="124"/>
-      <c r="G35" s="114"/>
-      <c r="I35" s="178" t="s">
+      <c r="B35" s="140"/>
+      <c r="C35" s="140"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="141"/>
+      <c r="G35" s="71"/>
+      <c r="I35" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="J35" s="179"/>
-      <c r="K35" s="179"/>
-      <c r="L35" s="179"/>
-      <c r="M35" s="179"/>
-      <c r="N35" s="180"/>
-      <c r="O35" s="177"/>
-    </row>
-    <row r="36" spans="1:15" ht="28.8">
-      <c r="A36" s="125" t="s">
+      <c r="J35" s="131"/>
+      <c r="K35" s="131"/>
+      <c r="L35" s="131"/>
+      <c r="M35" s="131"/>
+      <c r="N35" s="132"/>
+      <c r="O35" s="118"/>
+    </row>
+    <row r="36" spans="1:15" ht="43.75">
+      <c r="A36" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="126" t="s">
+      <c r="B36" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="127" t="s">
+      <c r="C36" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="127" t="s">
+      <c r="D36" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="127" t="s">
+      <c r="E36" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="128" t="s">
+      <c r="F36" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="114" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="175" t="s">
+      <c r="G36" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="J36" s="176" t="s">
+      <c r="J36" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="K36" s="176" t="s">
+      <c r="K36" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="L36" s="176" t="s">
+      <c r="L36" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="M36" s="176" t="s">
+      <c r="M36" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="N36" s="177" t="s">
+      <c r="N36" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="O36" s="177" t="s">
-        <v>28</v>
+      <c r="O36" s="118" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="129" t="s">
+      <c r="A37" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="130">
+      <c r="B37" s="81">
         <v>22344.329056898772</v>
       </c>
-      <c r="C37" s="131">
+      <c r="C37" s="82">
         <v>1</v>
       </c>
-      <c r="D37" s="132">
+      <c r="D37" s="83">
         <v>22344.329056898772</v>
       </c>
-      <c r="E37" s="132">
+      <c r="E37" s="83">
         <v>11766.199900161366</v>
       </c>
-      <c r="F37" s="133">
+      <c r="F37" s="84">
         <v>0</v>
       </c>
-      <c r="G37" s="114" t="s">
-        <v>25</v>
-      </c>
-      <c r="I37" s="175" t="s">
+      <c r="G37" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="J37" s="176">
+      <c r="J37" s="117">
         <v>7516273.5230968921</v>
       </c>
-      <c r="K37" s="176">
+      <c r="K37" s="117">
         <v>1</v>
       </c>
-      <c r="L37" s="176">
+      <c r="L37" s="117">
         <v>7516273.5230968921</v>
       </c>
-      <c r="M37" s="176">
+      <c r="M37" s="117">
         <v>0.68088794639577577</v>
       </c>
-      <c r="N37" s="177">
+      <c r="N37" s="118">
         <v>0.4093796362981551</v>
       </c>
-      <c r="O37" s="177" t="s">
+      <c r="O37" s="118" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="86">
+        <v>3794.2555654754333</v>
+      </c>
+      <c r="C38" s="87">
+        <v>1998</v>
+      </c>
+      <c r="D38" s="88">
+        <v>1.899026809547264</v>
+      </c>
+      <c r="E38" s="89"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="71"/>
+      <c r="I38" s="116" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="117">
+        <v>22055779631.056133</v>
+      </c>
+      <c r="K38" s="117">
+        <v>1998</v>
+      </c>
+      <c r="L38" s="117">
+        <v>11038928.744272338</v>
+      </c>
+      <c r="M38" s="117"/>
+      <c r="N38" s="118"/>
+      <c r="O38" s="118"/>
+    </row>
+    <row r="39" spans="1:15" ht="15" thickBot="1">
+      <c r="A39" s="114" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="115">
+        <v>26138.584622374205</v>
+      </c>
+      <c r="C39" s="91">
+        <v>1999</v>
+      </c>
+      <c r="D39" s="92"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="71"/>
+      <c r="I39" s="119" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="120">
+        <v>22063295904.579231</v>
+      </c>
+      <c r="K39" s="120">
+        <v>1999</v>
+      </c>
+      <c r="L39" s="120"/>
+      <c r="M39" s="120"/>
+      <c r="N39" s="121"/>
+      <c r="O39" s="118"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="75" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="70"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="71"/>
+      <c r="I40" s="116" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="117" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40" s="117"/>
+      <c r="L40" s="117"/>
+      <c r="M40" s="117"/>
+      <c r="N40" s="117"/>
+      <c r="O40" s="118"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="70"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="71"/>
+      <c r="I41" s="116" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" s="117" t="s">
+        <v>37</v>
+      </c>
+      <c r="K41" s="117"/>
+      <c r="L41" s="117"/>
+      <c r="M41" s="117"/>
+      <c r="N41" s="117"/>
+      <c r="O41" s="118"/>
+    </row>
+    <row r="42" spans="1:15" ht="28.2" customHeight="1">
+      <c r="A42" s="142" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="143"/>
+      <c r="C42" s="143"/>
+      <c r="D42" s="143"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="143"/>
+      <c r="G42" s="144"/>
+      <c r="I42" s="130" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="A38" s="134" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="135">
-        <v>3794.2555654754333</v>
-      </c>
-      <c r="C38" s="136">
-        <v>1998</v>
-      </c>
-      <c r="D38" s="137">
-        <v>1.899026809547264</v>
-      </c>
-      <c r="E38" s="138"/>
-      <c r="F38" s="139"/>
-      <c r="G38" s="114"/>
-      <c r="I38" s="175" t="s">
-        <v>20</v>
-      </c>
-      <c r="J38" s="176">
-        <v>22055779631.056133</v>
-      </c>
-      <c r="K38" s="176">
-        <v>1998</v>
-      </c>
-      <c r="L38" s="176">
-        <v>11038928.744272338</v>
-      </c>
-      <c r="M38" s="176"/>
-      <c r="N38" s="177"/>
-      <c r="O38" s="177"/>
-    </row>
-    <row r="39" spans="1:15" ht="14.7" thickBot="1">
-      <c r="A39" s="170" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="171">
-        <v>26138.584622374205</v>
-      </c>
-      <c r="C39" s="140">
-        <v>1999</v>
-      </c>
-      <c r="D39" s="141"/>
-      <c r="E39" s="141"/>
-      <c r="F39" s="142"/>
-      <c r="G39" s="114"/>
-      <c r="I39" s="187" t="s">
-        <v>8</v>
-      </c>
-      <c r="J39" s="188">
-        <v>22063295904.579231</v>
-      </c>
-      <c r="K39" s="188">
-        <v>1999</v>
-      </c>
-      <c r="L39" s="188"/>
-      <c r="M39" s="188"/>
-      <c r="N39" s="189"/>
-      <c r="O39" s="177"/>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="118" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="113" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="113"/>
-      <c r="D40" s="113"/>
-      <c r="E40" s="113"/>
-      <c r="F40" s="113"/>
-      <c r="G40" s="114"/>
-      <c r="I40" s="175" t="s">
-        <v>22</v>
-      </c>
-      <c r="J40" s="176" t="s">
-        <v>21</v>
-      </c>
-      <c r="K40" s="176"/>
-      <c r="L40" s="176"/>
-      <c r="M40" s="176"/>
-      <c r="N40" s="176"/>
-      <c r="O40" s="177"/>
-    </row>
-    <row r="41" spans="1:15">
-      <c r="A41" s="118" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="113" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="113"/>
-      <c r="D41" s="113"/>
-      <c r="E41" s="113"/>
-      <c r="F41" s="113"/>
-      <c r="G41" s="114"/>
-      <c r="I41" s="175" t="s">
-        <v>23</v>
-      </c>
-      <c r="J41" s="176" t="s">
-        <v>24</v>
-      </c>
-      <c r="K41" s="176"/>
-      <c r="L41" s="176"/>
-      <c r="M41" s="176"/>
-      <c r="N41" s="176"/>
-      <c r="O41" s="177"/>
-    </row>
-    <row r="42" spans="1:15" ht="28.2" customHeight="1">
-      <c r="A42" s="172" t="s">
+      <c r="J42" s="131"/>
+      <c r="K42" s="131"/>
+      <c r="L42" s="131"/>
+      <c r="M42" s="131"/>
+      <c r="N42" s="131"/>
+      <c r="O42" s="132"/>
+    </row>
+    <row r="43" spans="1:15" ht="16.2" customHeight="1">
+      <c r="A43" s="145" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="146"/>
+      <c r="C43" s="146"/>
+      <c r="D43" s="146"/>
+      <c r="E43" s="146"/>
+      <c r="F43" s="146"/>
+      <c r="G43" s="147"/>
+      <c r="I43" s="188" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="173"/>
-      <c r="C42" s="173"/>
-      <c r="D42" s="173"/>
-      <c r="E42" s="173"/>
-      <c r="F42" s="173"/>
-      <c r="G42" s="174"/>
-      <c r="I42" s="178" t="s">
-        <v>37</v>
-      </c>
-      <c r="J42" s="179"/>
-      <c r="K42" s="179"/>
-      <c r="L42" s="179"/>
-      <c r="M42" s="179"/>
-      <c r="N42" s="179"/>
-      <c r="O42" s="180"/>
-    </row>
-    <row r="43" spans="1:15" ht="16.2" customHeight="1">
-      <c r="A43" s="143" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="144"/>
-      <c r="C43" s="144"/>
-      <c r="D43" s="144"/>
-      <c r="E43" s="144"/>
-      <c r="F43" s="144"/>
-      <c r="G43" s="145"/>
-      <c r="I43" s="178" t="s">
-        <v>38</v>
-      </c>
-      <c r="J43" s="179"/>
-      <c r="K43" s="179"/>
-      <c r="L43" s="179"/>
-      <c r="M43" s="179"/>
-      <c r="N43" s="179"/>
-      <c r="O43" s="180"/>
-    </row>
-    <row r="44" spans="1:15" ht="29.1" customHeight="1" thickBot="1">
-      <c r="A44" s="146"/>
-      <c r="B44" s="147"/>
-      <c r="C44" s="147"/>
-      <c r="D44" s="147"/>
-      <c r="E44" s="147"/>
-      <c r="F44" s="147"/>
-      <c r="G44" s="148"/>
-      <c r="I44" s="181"/>
-      <c r="J44" s="182"/>
-      <c r="K44" s="182"/>
-      <c r="L44" s="182"/>
-      <c r="M44" s="182"/>
-      <c r="N44" s="182"/>
-      <c r="O44" s="183"/>
+      <c r="J43" s="189"/>
+      <c r="K43" s="189"/>
+      <c r="L43" s="189"/>
+      <c r="M43" s="189"/>
+      <c r="N43" s="189"/>
+      <c r="O43" s="190"/>
+    </row>
+    <row r="44" spans="1:15" ht="29.15" customHeight="1" thickBot="1">
+      <c r="A44" s="148"/>
+      <c r="B44" s="149"/>
+      <c r="C44" s="149"/>
+      <c r="D44" s="149"/>
+      <c r="E44" s="149"/>
+      <c r="F44" s="149"/>
+      <c r="G44" s="150"/>
+      <c r="I44" s="191"/>
+      <c r="J44" s="192"/>
+      <c r="K44" s="192"/>
+      <c r="L44" s="192"/>
+      <c r="M44" s="192"/>
+      <c r="N44" s="192"/>
+      <c r="O44" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A22:G23"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="I13:N13"/>
+    <mergeCell ref="I14:N14"/>
+    <mergeCell ref="I21:O21"/>
+    <mergeCell ref="I22:O23"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A43:G44"/>
     <mergeCell ref="I26:O26"/>
     <mergeCell ref="I34:N34"/>
     <mergeCell ref="I35:N35"/>
     <mergeCell ref="I42:O42"/>
     <mergeCell ref="I43:O44"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A43:G44"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="I13:N13"/>
-    <mergeCell ref="I14:N14"/>
-    <mergeCell ref="I21:O21"/>
-    <mergeCell ref="I22:O23"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A22:G23"/>
-    <mergeCell ref="A21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>